<commit_message>
add WeaponController to Character
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/DatasPath.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/DatasPath.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>RealTimePlayerData.xlsx</t>
+  </si>
+  <si>
+    <t>WeaponData</t>
+  </si>
+  <si>
+    <t>WeaponData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -379,6 +385,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update NPCPool and Instance role
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/DatasPath.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/DatasPath.xlsx
@@ -64,10 +64,10 @@
     <t>SceneProcessData.xlsx</t>
   </si>
   <si>
-    <t>PoolData</t>
-  </si>
-  <si>
-    <t>PoolData.xlsx</t>
+    <t>NPCPoolsData</t>
+  </si>
+  <si>
+    <t>NPCPoolsData.xlsx</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Update HPBar and add crystaldata, leveldata
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/DatasPath.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/DatasPath.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -64,10 +64,22 @@
     <t>SceneProcessData.xlsx</t>
   </si>
   <si>
-    <t>NPCPoolsData</t>
-  </si>
-  <si>
-    <t>NPCPoolsData.xlsx</t>
+    <t>NPCsData</t>
+  </si>
+  <si>
+    <t>NPCsData.xlsx</t>
+  </si>
+  <si>
+    <t>CrystalsData</t>
+  </si>
+  <si>
+    <t>CrystalsData.xlsx</t>
+  </si>
+  <si>
+    <t>LevelData</t>
+  </si>
+  <si>
+    <t>LevelData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -91,12 +103,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -111,14 +129,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -350,75 +371,91 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add item art resource and item can random push to game ui
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/DatasPath.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/DatasPath.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>LevelData.xlsx</t>
+  </si>
+  <si>
+    <t>ItemData</t>
+  </si>
+  <si>
+    <t>ItemData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -458,6 +464,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>